<commit_message>
increased owner name and date purchased with of cell on lot list report
</commit_message>
<xml_diff>
--- a/client/static/reports/lot_list/LOT_LIST_2016-12-05.xlsx
+++ b/client/static/reports/lot_list/LOT_LIST_2016-12-05.xlsx
@@ -1274,6 +1274,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="3" min="3" width="15"/>
+    <col customWidth="1" max="6" min="6" width="15"/>
+    <col customWidth="1" max="7" min="7" width="15"/>
+    <col customWidth="1" max="8" min="8" width="15"/>
+    <col customWidth="1" max="9" min="9" width="20"/>
+    <col customWidth="1" max="10" min="10" width="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">

</xml_diff>